<commit_message>
add Americas expansion birds and bonus
</commit_message>
<xml_diff>
--- a/scripts/wingspan-note-list.xlsx
+++ b/scripts/wingspan-note-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" state="visible" r:id="rId3"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="1090">
   <si>
     <t xml:space="preserve">Common name</t>
   </si>
@@ -2121,35 +2121,7 @@
     <t xml:space="preserve">Rifleman</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">T</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ī</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">tipounamu</t>
-    </r>
+    <t xml:space="preserve">Tītipounamu</t>
   </si>
   <si>
     <t xml:space="preserve">Shore Plover</t>
@@ -2955,6 +2927,224 @@
     <t xml:space="preserve">Count how many unspent food tokens you have at the end of the game. Food cached on birds does not count as part of your supply.</t>
   </si>
   <si>
+    <t xml:space="preserve">Hummingbird Gardener</t>
+  </si>
+  <si>
+    <t xml:space="preserve">americas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hummingbird tokens worth at least 4 points</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[point]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> each</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Hummingbird Counter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[hummingbird] spaces that you reached on your hummingbird track</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[point]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> each</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Apiarist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point value of your [bee] token</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">3 to 4 points: 3[point]; 6 to 8 points: 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[point]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; 10 points: 6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[point]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Brilliant Specialist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point value of your [brilliant] token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emerald Specialist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point value of your [emerald] token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mango Specialist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point value of your [mango] token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topaz Specialist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point value of your [topaz] token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecolodge Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Score more if your hummingbirds are close in value. Compare the points values of your highest and lowest tokens. If the difference is:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">0 to 2 points: 6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[point]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; 3 points: 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[point]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; 4+ points: 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[point]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[automa] Charm Champion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds with “Hummingbird” in their power or name</t>
+  </si>
+  <si>
     <t xml:space="preserve">Goal</t>
   </si>
   <si>
@@ -3349,7 +3539,7 @@
     <numFmt numFmtId="166" formatCode="&quot;PRAWDA&quot;;&quot;PRAWDA&quot;;&quot;FAŁSZ&quot;"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3410,12 +3600,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -3450,6 +3634,26 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -3495,7 +3699,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3544,12 +3748,28 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -3557,22 +3777,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3584,23 +3788,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3608,7 +3824,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3766,7 +3982,7 @@
   </sheetPr>
   <dimension ref="A1:C1597"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B524" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -12437,12 +12653,12 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="G56" activeCellId="0" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14012,57 +14228,216 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C54" s="6"/>
+      <c r="A54" s="1" t="n">
+        <v>1050</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>939</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D54" s="6"/>
-      <c r="H54" s="23"/>
-      <c r="J54" s="21"/>
+      <c r="E54" s="26" t="s">
+        <v>941</v>
+      </c>
+      <c r="G54" s="27" t="s">
+        <v>942</v>
+      </c>
+      <c r="H54" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J54" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C55" s="6"/>
+      <c r="A55" s="1" t="n">
+        <v>1051</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>943</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D55" s="6"/>
-      <c r="H55" s="23"/>
-      <c r="J55" s="21"/>
+      <c r="E55" s="26" t="s">
+        <v>944</v>
+      </c>
+      <c r="G55" s="26" t="s">
+        <v>945</v>
+      </c>
+      <c r="H55" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J55" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C56" s="6"/>
+      <c r="A56" s="1" t="n">
+        <v>1052</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>946</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D56" s="6"/>
-      <c r="H56" s="23"/>
-      <c r="J56" s="21"/>
+      <c r="E56" s="26" t="s">
+        <v>947</v>
+      </c>
+      <c r="G56" s="27" t="s">
+        <v>948</v>
+      </c>
+      <c r="H56" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J56" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C57" s="6"/>
+      <c r="A57" s="1" t="n">
+        <v>1053</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>949</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D57" s="6"/>
-      <c r="H57" s="23"/>
-      <c r="J57" s="21"/>
+      <c r="E57" s="26" t="s">
+        <v>950</v>
+      </c>
+      <c r="G57" s="27" t="s">
+        <v>948</v>
+      </c>
+      <c r="H57" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J57" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C58" s="6"/>
+      <c r="A58" s="1" t="n">
+        <v>1054</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>951</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D58" s="6"/>
-      <c r="H58" s="23"/>
-      <c r="J58" s="21"/>
+      <c r="E58" s="26" t="s">
+        <v>952</v>
+      </c>
+      <c r="G58" s="27" t="s">
+        <v>948</v>
+      </c>
+      <c r="H58" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J58" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C59" s="6"/>
+      <c r="A59" s="1" t="n">
+        <v>1055</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>953</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D59" s="6"/>
-      <c r="H59" s="23"/>
-      <c r="J59" s="21"/>
+      <c r="E59" s="26" t="s">
+        <v>954</v>
+      </c>
+      <c r="G59" s="27" t="s">
+        <v>948</v>
+      </c>
+      <c r="H59" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J59" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C60" s="6"/>
+      <c r="A60" s="1" t="n">
+        <v>1056</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>955</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D60" s="6"/>
-      <c r="H60" s="23"/>
-      <c r="J60" s="21"/>
+      <c r="E60" s="26" t="s">
+        <v>956</v>
+      </c>
+      <c r="G60" s="27" t="s">
+        <v>948</v>
+      </c>
+      <c r="H60" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J60" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C61" s="6"/>
+      <c r="A61" s="1" t="n">
+        <v>1057</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>957</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D61" s="6"/>
-      <c r="H61" s="23"/>
-      <c r="J61" s="21"/>
+      <c r="E61" s="26" t="s">
+        <v>958</v>
+      </c>
+      <c r="G61" s="27" t="s">
+        <v>959</v>
+      </c>
+      <c r="H61" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J61" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="H62" s="23"/>
+      <c r="A62" s="1" t="n">
+        <v>1058</v>
+      </c>
+      <c r="B62" s="28" t="s">
+        <v>960</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>940</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>758</v>
+      </c>
+      <c r="E62" s="28" t="s">
+        <v>961</v>
+      </c>
+      <c r="H62" s="23" t="s">
+        <v>782</v>
+      </c>
       <c r="J62" s="21"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19733,897 +20108,897 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>747</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>939</v>
-      </c>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="29" t="s">
+        <v>962</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>749</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>940</v>
-      </c>
-      <c r="E1" s="26" t="s">
+      <c r="D1" s="29" t="s">
+        <v>963</v>
+      </c>
+      <c r="E1" s="29" t="s">
         <v>751</v>
       </c>
-      <c r="F1" s="26" t="s">
-        <v>941</v>
-      </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
+      <c r="F1" s="29" t="s">
+        <v>964</v>
+      </c>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="n">
+      <c r="A2" s="29" t="n">
         <v>2000</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>942</v>
-      </c>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="29" t="s">
+        <v>965</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26" t="s">
-        <v>943</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>944</v>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29" t="s">
+        <v>966</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>967</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="n">
+      <c r="A3" s="29" t="n">
         <v>2001</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>945</v>
-      </c>
-      <c r="C3" s="26" t="s">
+      <c r="B3" s="29" t="s">
+        <v>968</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26" t="s">
-        <v>946</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>944</v>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29" t="s">
+        <v>969</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>967</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="n">
+      <c r="A4" s="29" t="n">
         <v>2002</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>947</v>
-      </c>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="29" t="s">
+        <v>970</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26" t="s">
-        <v>948</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>944</v>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29" t="s">
+        <v>971</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>967</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="25" t="n">
         <v>2013</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>949</v>
-      </c>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="29" t="s">
+        <v>972</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26" t="s">
-        <v>950</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>951</v>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29" t="s">
+        <v>973</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>974</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="25" t="n">
         <v>2014</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>952</v>
-      </c>
-      <c r="C6" s="26" t="s">
+      <c r="B6" s="29" t="s">
+        <v>975</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26" t="s">
-        <v>953</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>951</v>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29" t="s">
+        <v>976</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>974</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="25" t="n">
         <v>2017</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>954</v>
-      </c>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="29" t="s">
+        <v>977</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26" t="s">
-        <v>955</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>951</v>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29" t="s">
+        <v>978</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>974</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="25" t="n">
         <v>2010</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>956</v>
-      </c>
-      <c r="C8" s="26" t="s">
+      <c r="B8" s="29" t="s">
+        <v>979</v>
+      </c>
+      <c r="C8" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26" t="s">
-        <v>957</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>958</v>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29" t="s">
+        <v>980</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>981</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="25" t="n">
         <v>2008</v>
       </c>
-      <c r="B9" s="26" t="s">
-        <v>959</v>
-      </c>
-      <c r="C9" s="26" t="s">
+      <c r="B9" s="29" t="s">
+        <v>982</v>
+      </c>
+      <c r="C9" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26" t="s">
-        <v>960</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>958</v>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29" t="s">
+        <v>983</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>981</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="25" t="n">
         <v>2021</v>
       </c>
-      <c r="B10" s="26" t="s">
-        <v>961</v>
-      </c>
-      <c r="C10" s="26" t="s">
+      <c r="B10" s="29" t="s">
+        <v>984</v>
+      </c>
+      <c r="C10" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26" t="s">
-        <v>962</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>958</v>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29" t="s">
+        <v>985</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>981</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="25" t="n">
         <v>2022</v>
       </c>
-      <c r="B11" s="26" t="s">
-        <v>963</v>
-      </c>
-      <c r="C11" s="26" t="s">
+      <c r="B11" s="29" t="s">
+        <v>986</v>
+      </c>
+      <c r="C11" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26" t="s">
-        <v>964</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>965</v>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29" t="s">
+        <v>987</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>988</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="25" t="n">
         <v>2012</v>
       </c>
-      <c r="B12" s="26" t="s">
-        <v>966</v>
-      </c>
-      <c r="C12" s="26" t="s">
+      <c r="B12" s="29" t="s">
+        <v>989</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26" t="s">
-        <v>967</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>965</v>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29" t="s">
+        <v>990</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>988</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="25" t="n">
         <v>2011</v>
       </c>
-      <c r="B13" s="26" t="s">
-        <v>968</v>
-      </c>
-      <c r="C13" s="26" t="s">
+      <c r="B13" s="29" t="s">
+        <v>991</v>
+      </c>
+      <c r="C13" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26" t="s">
-        <v>969</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>965</v>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29" t="s">
+        <v>992</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>988</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="25" t="n">
         <v>2015</v>
       </c>
-      <c r="B14" s="26" t="s">
-        <v>970</v>
-      </c>
-      <c r="C14" s="26" t="s">
+      <c r="B14" s="29" t="s">
+        <v>993</v>
+      </c>
+      <c r="C14" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26" t="s">
-        <v>971</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>965</v>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29" t="s">
+        <v>994</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>988</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="25" t="n">
         <v>2016</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>972</v>
-      </c>
-      <c r="C15" s="26" t="s">
+      <c r="B15" s="29" t="s">
+        <v>995</v>
+      </c>
+      <c r="C15" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26" t="s">
-        <v>973</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>965</v>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29" t="s">
+        <v>996</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>988</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="25" t="n">
         <v>2023</v>
       </c>
-      <c r="B16" s="26" t="s">
-        <v>974</v>
-      </c>
-      <c r="C16" s="26" t="s">
+      <c r="B16" s="29" t="s">
+        <v>997</v>
+      </c>
+      <c r="C16" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26" t="s">
-        <v>975</v>
-      </c>
-      <c r="F16" s="26" t="s">
-        <v>976</v>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29" t="s">
+        <v>998</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>999</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="25" t="n">
         <v>2024</v>
       </c>
-      <c r="B17" s="26" t="s">
-        <v>977</v>
-      </c>
-      <c r="C17" s="26" t="s">
+      <c r="B17" s="29" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26" t="s">
-        <v>978</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>979</v>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>1002</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="25" t="n">
         <v>2020</v>
       </c>
-      <c r="B18" s="26" t="s">
-        <v>980</v>
-      </c>
-      <c r="C18" s="26" t="s">
+      <c r="B18" s="29" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26" t="s">
-        <v>981</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>982</v>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>1005</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26" t="n">
+      <c r="A19" s="29" t="n">
         <v>2003</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>983</v>
-      </c>
-      <c r="C19" s="26" t="s">
+      <c r="B19" s="29" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26" t="s">
-        <v>984</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>985</v>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F19" s="29" t="s">
+        <v>1008</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="25" t="n">
         <v>2004</v>
       </c>
-      <c r="B20" s="26" t="s">
-        <v>986</v>
-      </c>
-      <c r="C20" s="26" t="s">
+      <c r="B20" s="29" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C20" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26" t="s">
-        <v>987</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>988</v>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>1011</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="25" t="n">
         <v>2006</v>
       </c>
-      <c r="B21" s="26" t="s">
-        <v>989</v>
-      </c>
-      <c r="C21" s="26" t="s">
+      <c r="B21" s="29" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C21" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26" t="s">
-        <v>990</v>
-      </c>
-      <c r="F21" s="26" t="s">
-        <v>991</v>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>1014</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="25" t="n">
         <v>2005</v>
       </c>
-      <c r="B22" s="26" t="s">
-        <v>992</v>
-      </c>
-      <c r="C22" s="26" t="s">
+      <c r="B22" s="29" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C22" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26" t="s">
-        <v>993</v>
-      </c>
-      <c r="F22" s="26" t="s">
-        <v>994</v>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29" t="s">
+        <v>1016</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>1017</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="25" t="n">
         <v>2018</v>
       </c>
-      <c r="B23" s="26" t="s">
-        <v>995</v>
-      </c>
-      <c r="C23" s="26" t="s">
+      <c r="B23" s="29" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C23" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26" t="s">
-        <v>996</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>997</v>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>1020</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="25" t="n">
         <v>2009</v>
       </c>
-      <c r="B24" s="26" t="s">
-        <v>998</v>
-      </c>
-      <c r="C24" s="26" t="s">
+      <c r="B24" s="29" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C24" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26" t="s">
-        <v>999</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>1000</v>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>1023</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="25" t="n">
         <v>2025</v>
       </c>
-      <c r="B25" s="26" t="s">
-        <v>1001</v>
-      </c>
-      <c r="C25" s="26" t="s">
+      <c r="B25" s="29" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C25" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26" t="s">
-        <v>1002</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>1003</v>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>1026</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="25" t="n">
         <v>2007</v>
       </c>
-      <c r="B26" s="26" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C26" s="26" t="s">
+      <c r="B26" s="29" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C26" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26" t="s">
-        <v>1005</v>
-      </c>
-      <c r="F26" s="26" t="s">
-        <v>1006</v>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>1029</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="25" t="n">
         <v>2019</v>
       </c>
-      <c r="B27" s="26" t="s">
-        <v>1007</v>
-      </c>
-      <c r="C27" s="26" t="s">
+      <c r="B27" s="29" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C27" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26" t="s">
-        <v>1008</v>
-      </c>
-      <c r="F27" s="26" t="s">
-        <v>1009</v>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>1032</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="25" t="n">
         <v>2031</v>
       </c>
-      <c r="B28" s="26" t="s">
-        <v>1010</v>
-      </c>
-      <c r="C28" s="26" t="s">
+      <c r="B28" s="29" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C28" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26" t="s">
-        <v>1011</v>
-      </c>
-      <c r="F28" s="26" t="s">
-        <v>1012</v>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>1035</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="25" t="n">
         <v>2030</v>
       </c>
-      <c r="B29" s="26" t="s">
-        <v>1013</v>
-      </c>
-      <c r="C29" s="26" t="s">
+      <c r="B29" s="29" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C29" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26" t="s">
-        <v>1014</v>
-      </c>
-      <c r="F29" s="26" t="s">
-        <v>1012</v>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>1035</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="25" t="n">
         <v>2033</v>
       </c>
-      <c r="B30" s="26" t="s">
-        <v>1015</v>
-      </c>
-      <c r="C30" s="26" t="s">
+      <c r="B30" s="29" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C30" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26" t="s">
-        <v>1016</v>
-      </c>
-      <c r="F30" s="26" t="s">
-        <v>1012</v>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>1035</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="25" t="n">
         <v>2032</v>
       </c>
-      <c r="B31" s="26" t="s">
-        <v>1017</v>
-      </c>
-      <c r="C31" s="26" t="s">
+      <c r="B31" s="29" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C31" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26" t="s">
-        <v>1018</v>
-      </c>
-      <c r="F31" s="26" t="s">
-        <v>1019</v>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>1042</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="25" t="n">
         <v>2026</v>
       </c>
-      <c r="B32" s="26" t="s">
-        <v>1020</v>
-      </c>
-      <c r="C32" s="26" t="s">
+      <c r="B32" s="29" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C32" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26" t="s">
-        <v>1021</v>
-      </c>
-      <c r="F32" s="26" t="s">
-        <v>1022</v>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F32" s="29" t="s">
+        <v>1045</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="25" t="n">
         <v>2027</v>
       </c>
-      <c r="B33" s="26" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C33" s="26" t="s">
+      <c r="B33" s="29" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C33" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26" t="s">
-        <v>1024</v>
-      </c>
-      <c r="F33" s="26" t="s">
-        <v>1022</v>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F33" s="29" t="s">
+        <v>1045</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="25" t="n">
         <v>2029</v>
       </c>
-      <c r="B34" s="26" t="s">
-        <v>1025</v>
-      </c>
-      <c r="C34" s="26" t="s">
+      <c r="B34" s="29" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C34" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26" t="s">
-        <v>1026</v>
-      </c>
-      <c r="F34" s="26" t="s">
-        <v>1027</v>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29" t="s">
+        <v>1049</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>1050</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="25" t="n">
         <v>2028</v>
       </c>
-      <c r="B35" s="26" t="s">
-        <v>1028</v>
-      </c>
-      <c r="C35" s="26" t="s">
+      <c r="B35" s="29" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C35" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26" t="s">
-        <v>1029</v>
-      </c>
-      <c r="F35" s="26" t="s">
-        <v>1030</v>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29" t="s">
+        <v>1052</v>
+      </c>
+      <c r="F35" s="29" t="s">
+        <v>1053</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="25" t="n">
         <v>2043</v>
       </c>
-      <c r="B36" s="26" t="s">
-        <v>1031</v>
-      </c>
-      <c r="C36" s="26" t="s">
+      <c r="B36" s="29" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C36" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D36" s="26" t="s">
+      <c r="D36" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E36" s="26" t="s">
-        <v>1032</v>
-      </c>
-      <c r="F36" s="26" t="s">
-        <v>1033</v>
+      <c r="E36" s="29" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>1056</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="25" t="n">
         <v>2040</v>
       </c>
-      <c r="B37" s="26" t="s">
-        <v>1034</v>
-      </c>
-      <c r="C37" s="26" t="s">
+      <c r="B37" s="29" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C37" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D37" s="26" t="s">
+      <c r="D37" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E37" s="26" t="s">
-        <v>1035</v>
-      </c>
-      <c r="F37" s="26" t="s">
-        <v>1036</v>
+      <c r="E37" s="29" t="s">
+        <v>1058</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>1059</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="25" t="n">
         <v>2035</v>
       </c>
-      <c r="B38" s="26" t="s">
-        <v>1037</v>
-      </c>
-      <c r="C38" s="26" t="s">
+      <c r="B38" s="29" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C38" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D38" s="26" t="s">
+      <c r="D38" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E38" s="26" t="s">
-        <v>1038</v>
-      </c>
-      <c r="F38" s="26" t="s">
-        <v>1039</v>
+      <c r="E38" s="29" t="s">
+        <v>1061</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>1062</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="25" t="n">
         <v>2041</v>
       </c>
-      <c r="B39" s="26" t="s">
-        <v>1040</v>
-      </c>
-      <c r="C39" s="26" t="s">
+      <c r="B39" s="29" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C39" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D39" s="26" t="s">
+      <c r="D39" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E39" s="26" t="s">
-        <v>1041</v>
-      </c>
-      <c r="F39" s="26" t="s">
-        <v>1042</v>
+      <c r="E39" s="29" t="s">
+        <v>1064</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>1065</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="25" t="n">
         <v>2042</v>
       </c>
-      <c r="B40" s="26" t="s">
-        <v>1043</v>
-      </c>
-      <c r="C40" s="26" t="s">
+      <c r="B40" s="29" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C40" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D40" s="26" t="s">
+      <c r="D40" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E40" s="26" t="s">
-        <v>1044</v>
-      </c>
-      <c r="F40" s="26" t="s">
-        <v>1042</v>
+      <c r="E40" s="29" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F40" s="29" t="s">
+        <v>1065</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="25" t="n">
         <v>2044</v>
       </c>
-      <c r="B41" s="26" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C41" s="26" t="s">
+      <c r="B41" s="29" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C41" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D41" s="26" t="s">
+      <c r="D41" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E41" s="26" t="s">
-        <v>1046</v>
-      </c>
-      <c r="F41" s="26" t="s">
-        <v>1047</v>
+      <c r="E41" s="29" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>1070</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="25" t="n">
         <v>2036</v>
       </c>
-      <c r="B42" s="26" t="s">
-        <v>1048</v>
-      </c>
-      <c r="C42" s="26" t="s">
+      <c r="B42" s="29" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C42" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D42" s="26" t="s">
+      <c r="D42" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E42" s="26" t="s">
-        <v>1049</v>
-      </c>
-      <c r="F42" s="26" t="s">
-        <v>1050</v>
+      <c r="E42" s="29" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>1073</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="25" t="n">
         <v>2034</v>
       </c>
-      <c r="B43" s="26" t="s">
-        <v>1051</v>
-      </c>
-      <c r="C43" s="26" t="s">
+      <c r="B43" s="29" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C43" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D43" s="26" t="s">
+      <c r="D43" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E43" s="26" t="s">
-        <v>1052</v>
-      </c>
-      <c r="F43" s="26" t="s">
-        <v>1053</v>
+      <c r="E43" s="29" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>1076</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="25" t="n">
         <v>2037</v>
       </c>
-      <c r="B44" s="26" t="s">
-        <v>1054</v>
-      </c>
-      <c r="C44" s="26" t="s">
+      <c r="B44" s="29" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C44" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D44" s="26" t="s">
+      <c r="D44" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E44" s="26" t="s">
-        <v>1055</v>
-      </c>
-      <c r="F44" s="26" t="s">
-        <v>1056</v>
+      <c r="E44" s="29" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>1079</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="25" t="n">
         <v>2038</v>
       </c>
-      <c r="B45" s="26" t="s">
-        <v>1057</v>
-      </c>
-      <c r="C45" s="26" t="s">
+      <c r="B45" s="29" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C45" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D45" s="26" t="s">
+      <c r="D45" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E45" s="26" t="s">
-        <v>1058</v>
-      </c>
-      <c r="F45" s="26" t="s">
-        <v>1056</v>
+      <c r="E45" s="29" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>1079</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="25" t="n">
         <v>2039</v>
       </c>
-      <c r="B46" s="26" t="s">
-        <v>1059</v>
-      </c>
-      <c r="C46" s="26" t="s">
+      <c r="B46" s="29" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C46" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D46" s="26" t="s">
+      <c r="D46" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E46" s="26" t="s">
-        <v>1060</v>
-      </c>
-      <c r="F46" s="26" t="s">
-        <v>1056</v>
+      <c r="E46" s="29" t="s">
+        <v>1083</v>
+      </c>
+      <c r="F46" s="29" t="s">
+        <v>1079</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="25" t="n">
         <v>2045</v>
       </c>
-      <c r="B47" s="26" t="s">
-        <v>1061</v>
-      </c>
-      <c r="C47" s="26" t="s">
+      <c r="B47" s="29" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C47" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D47" s="26" t="s">
+      <c r="D47" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E47" s="26" t="s">
-        <v>1062</v>
-      </c>
-      <c r="F47" s="26" t="s">
-        <v>1063</v>
+      <c r="E47" s="29" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F47" s="29" t="s">
+        <v>1086</v>
       </c>
     </row>
   </sheetData>
@@ -20655,22 +21030,22 @@
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
-        <v>1064</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>1065</v>
+      <c r="A1" s="29" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>1088</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>1066</v>
-      </c>
-      <c r="B2" s="27" t="n">
+      <c r="A2" s="29" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B2" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
add Americas expansion birds and bonus (#102)
* add Americas expansion birds and bonus

* sync spreadsheet, add default hummingbird values

* update hummingbirds, basic skeleton display

* Add Hummingbird detail view, Polish UI, Add bird silhouettes

* Add americas expansion icon

* Publish changes

---------

Co-authored-by: Matej Cief <cief@amazon.co.uk>
Co-authored-by: Matej Cief <matej.cief@gmail.com>
</commit_message>
<xml_diff>
--- a/scripts/wingspan-note-list.xlsx
+++ b/scripts/wingspan-note-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" state="visible" r:id="rId3"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="1090">
   <si>
     <t xml:space="preserve">Common name</t>
   </si>
@@ -2121,35 +2121,7 @@
     <t xml:space="preserve">Rifleman</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">T</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">ī</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">tipounamu</t>
-    </r>
+    <t xml:space="preserve">Tītipounamu</t>
   </si>
   <si>
     <t xml:space="preserve">Shore Plover</t>
@@ -2955,6 +2927,224 @@
     <t xml:space="preserve">Count how many unspent food tokens you have at the end of the game. Food cached on birds does not count as part of your supply.</t>
   </si>
   <si>
+    <t xml:space="preserve">Hummingbird Gardener</t>
+  </si>
+  <si>
+    <t xml:space="preserve">americas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hummingbird tokens worth at least 4 points</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[point]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> each</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Hummingbird Counter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[hummingbird] spaces that you reached on your hummingbird track</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[point]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> each</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Apiarist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point value of your [bee] token</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">3 to 4 points: 3[point]; 6 to 8 points: 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[point]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; 10 points: 6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[point]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Brilliant Specialist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point value of your [brilliant] token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emerald Specialist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point value of your [emerald] token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mango Specialist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point value of your [mango] token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topaz Specialist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point value of your [topaz] token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecolodge Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Score more if your hummingbirds are close in value. Compare the points values of your highest and lowest tokens. If the difference is:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">0 to 2 points: 6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[point]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; 3 points: 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[point]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; 4+ points: 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">[point]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[automa] Charm Champion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds with “Hummingbird” in their power or name</t>
+  </si>
+  <si>
     <t xml:space="preserve">Goal</t>
   </si>
   <si>
@@ -3349,7 +3539,7 @@
     <numFmt numFmtId="166" formatCode="&quot;PRAWDA&quot;;&quot;PRAWDA&quot;;&quot;FAŁSZ&quot;"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3410,12 +3600,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -3450,6 +3634,26 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -3495,7 +3699,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3544,12 +3748,28 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -3557,22 +3777,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3584,23 +3788,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3608,7 +3824,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3766,7 +3982,7 @@
   </sheetPr>
   <dimension ref="A1:C1597"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B524" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -12437,12 +12653,12 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="G56" activeCellId="0" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14012,57 +14228,216 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C54" s="6"/>
+      <c r="A54" s="1" t="n">
+        <v>1050</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>939</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D54" s="6"/>
-      <c r="H54" s="23"/>
-      <c r="J54" s="21"/>
+      <c r="E54" s="26" t="s">
+        <v>941</v>
+      </c>
+      <c r="G54" s="27" t="s">
+        <v>942</v>
+      </c>
+      <c r="H54" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J54" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C55" s="6"/>
+      <c r="A55" s="1" t="n">
+        <v>1051</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>943</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D55" s="6"/>
-      <c r="H55" s="23"/>
-      <c r="J55" s="21"/>
+      <c r="E55" s="26" t="s">
+        <v>944</v>
+      </c>
+      <c r="G55" s="26" t="s">
+        <v>945</v>
+      </c>
+      <c r="H55" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J55" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C56" s="6"/>
+      <c r="A56" s="1" t="n">
+        <v>1052</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>946</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D56" s="6"/>
-      <c r="H56" s="23"/>
-      <c r="J56" s="21"/>
+      <c r="E56" s="26" t="s">
+        <v>947</v>
+      </c>
+      <c r="G56" s="27" t="s">
+        <v>948</v>
+      </c>
+      <c r="H56" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J56" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C57" s="6"/>
+      <c r="A57" s="1" t="n">
+        <v>1053</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>949</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D57" s="6"/>
-      <c r="H57" s="23"/>
-      <c r="J57" s="21"/>
+      <c r="E57" s="26" t="s">
+        <v>950</v>
+      </c>
+      <c r="G57" s="27" t="s">
+        <v>948</v>
+      </c>
+      <c r="H57" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J57" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C58" s="6"/>
+      <c r="A58" s="1" t="n">
+        <v>1054</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>951</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D58" s="6"/>
-      <c r="H58" s="23"/>
-      <c r="J58" s="21"/>
+      <c r="E58" s="26" t="s">
+        <v>952</v>
+      </c>
+      <c r="G58" s="27" t="s">
+        <v>948</v>
+      </c>
+      <c r="H58" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J58" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C59" s="6"/>
+      <c r="A59" s="1" t="n">
+        <v>1055</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>953</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D59" s="6"/>
-      <c r="H59" s="23"/>
-      <c r="J59" s="21"/>
+      <c r="E59" s="26" t="s">
+        <v>954</v>
+      </c>
+      <c r="G59" s="27" t="s">
+        <v>948</v>
+      </c>
+      <c r="H59" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J59" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C60" s="6"/>
+      <c r="A60" s="1" t="n">
+        <v>1056</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>955</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D60" s="6"/>
-      <c r="H60" s="23"/>
-      <c r="J60" s="21"/>
+      <c r="E60" s="26" t="s">
+        <v>956</v>
+      </c>
+      <c r="G60" s="27" t="s">
+        <v>948</v>
+      </c>
+      <c r="H60" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J60" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C61" s="6"/>
+      <c r="A61" s="1" t="n">
+        <v>1057</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>957</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="D61" s="6"/>
-      <c r="H61" s="23"/>
-      <c r="J61" s="21"/>
+      <c r="E61" s="26" t="s">
+        <v>958</v>
+      </c>
+      <c r="G61" s="27" t="s">
+        <v>959</v>
+      </c>
+      <c r="H61" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="J61" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="H62" s="23"/>
+      <c r="A62" s="1" t="n">
+        <v>1058</v>
+      </c>
+      <c r="B62" s="28" t="s">
+        <v>960</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>940</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>758</v>
+      </c>
+      <c r="E62" s="28" t="s">
+        <v>961</v>
+      </c>
+      <c r="H62" s="23" t="s">
+        <v>782</v>
+      </c>
       <c r="J62" s="21"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19733,897 +20108,897 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>747</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>939</v>
-      </c>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="29" t="s">
+        <v>962</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>749</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>940</v>
-      </c>
-      <c r="E1" s="26" t="s">
+      <c r="D1" s="29" t="s">
+        <v>963</v>
+      </c>
+      <c r="E1" s="29" t="s">
         <v>751</v>
       </c>
-      <c r="F1" s="26" t="s">
-        <v>941</v>
-      </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
+      <c r="F1" s="29" t="s">
+        <v>964</v>
+      </c>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="n">
+      <c r="A2" s="29" t="n">
         <v>2000</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>942</v>
-      </c>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="29" t="s">
+        <v>965</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26" t="s">
-        <v>943</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>944</v>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29" t="s">
+        <v>966</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>967</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="n">
+      <c r="A3" s="29" t="n">
         <v>2001</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>945</v>
-      </c>
-      <c r="C3" s="26" t="s">
+      <c r="B3" s="29" t="s">
+        <v>968</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26" t="s">
-        <v>946</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>944</v>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29" t="s">
+        <v>969</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>967</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="n">
+      <c r="A4" s="29" t="n">
         <v>2002</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>947</v>
-      </c>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="29" t="s">
+        <v>970</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26" t="s">
-        <v>948</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>944</v>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29" t="s">
+        <v>971</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>967</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="25" t="n">
         <v>2013</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>949</v>
-      </c>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="29" t="s">
+        <v>972</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26" t="s">
-        <v>950</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>951</v>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29" t="s">
+        <v>973</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>974</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="25" t="n">
         <v>2014</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>952</v>
-      </c>
-      <c r="C6" s="26" t="s">
+      <c r="B6" s="29" t="s">
+        <v>975</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26" t="s">
-        <v>953</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>951</v>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29" t="s">
+        <v>976</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>974</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="25" t="n">
         <v>2017</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>954</v>
-      </c>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="29" t="s">
+        <v>977</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26" t="s">
-        <v>955</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>951</v>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29" t="s">
+        <v>978</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>974</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="25" t="n">
         <v>2010</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>956</v>
-      </c>
-      <c r="C8" s="26" t="s">
+      <c r="B8" s="29" t="s">
+        <v>979</v>
+      </c>
+      <c r="C8" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26" t="s">
-        <v>957</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>958</v>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29" t="s">
+        <v>980</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>981</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="25" t="n">
         <v>2008</v>
       </c>
-      <c r="B9" s="26" t="s">
-        <v>959</v>
-      </c>
-      <c r="C9" s="26" t="s">
+      <c r="B9" s="29" t="s">
+        <v>982</v>
+      </c>
+      <c r="C9" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26" t="s">
-        <v>960</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>958</v>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29" t="s">
+        <v>983</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>981</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="25" t="n">
         <v>2021</v>
       </c>
-      <c r="B10" s="26" t="s">
-        <v>961</v>
-      </c>
-      <c r="C10" s="26" t="s">
+      <c r="B10" s="29" t="s">
+        <v>984</v>
+      </c>
+      <c r="C10" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26" t="s">
-        <v>962</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>958</v>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29" t="s">
+        <v>985</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>981</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="25" t="n">
         <v>2022</v>
       </c>
-      <c r="B11" s="26" t="s">
-        <v>963</v>
-      </c>
-      <c r="C11" s="26" t="s">
+      <c r="B11" s="29" t="s">
+        <v>986</v>
+      </c>
+      <c r="C11" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26" t="s">
-        <v>964</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>965</v>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29" t="s">
+        <v>987</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>988</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="25" t="n">
         <v>2012</v>
       </c>
-      <c r="B12" s="26" t="s">
-        <v>966</v>
-      </c>
-      <c r="C12" s="26" t="s">
+      <c r="B12" s="29" t="s">
+        <v>989</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26" t="s">
-        <v>967</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>965</v>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29" t="s">
+        <v>990</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>988</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="25" t="n">
         <v>2011</v>
       </c>
-      <c r="B13" s="26" t="s">
-        <v>968</v>
-      </c>
-      <c r="C13" s="26" t="s">
+      <c r="B13" s="29" t="s">
+        <v>991</v>
+      </c>
+      <c r="C13" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26" t="s">
-        <v>969</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>965</v>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29" t="s">
+        <v>992</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>988</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="25" t="n">
         <v>2015</v>
       </c>
-      <c r="B14" s="26" t="s">
-        <v>970</v>
-      </c>
-      <c r="C14" s="26" t="s">
+      <c r="B14" s="29" t="s">
+        <v>993</v>
+      </c>
+      <c r="C14" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26" t="s">
-        <v>971</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>965</v>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29" t="s">
+        <v>994</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>988</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="25" t="n">
         <v>2016</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>972</v>
-      </c>
-      <c r="C15" s="26" t="s">
+      <c r="B15" s="29" t="s">
+        <v>995</v>
+      </c>
+      <c r="C15" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26" t="s">
-        <v>973</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>965</v>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29" t="s">
+        <v>996</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>988</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="25" t="n">
         <v>2023</v>
       </c>
-      <c r="B16" s="26" t="s">
-        <v>974</v>
-      </c>
-      <c r="C16" s="26" t="s">
+      <c r="B16" s="29" t="s">
+        <v>997</v>
+      </c>
+      <c r="C16" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26" t="s">
-        <v>975</v>
-      </c>
-      <c r="F16" s="26" t="s">
-        <v>976</v>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29" t="s">
+        <v>998</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>999</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="25" t="n">
         <v>2024</v>
       </c>
-      <c r="B17" s="26" t="s">
-        <v>977</v>
-      </c>
-      <c r="C17" s="26" t="s">
+      <c r="B17" s="29" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>757</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26" t="s">
-        <v>978</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>979</v>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>1002</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="25" t="n">
         <v>2020</v>
       </c>
-      <c r="B18" s="26" t="s">
-        <v>980</v>
-      </c>
-      <c r="C18" s="26" t="s">
+      <c r="B18" s="29" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26" t="s">
-        <v>981</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>982</v>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>1005</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26" t="n">
+      <c r="A19" s="29" t="n">
         <v>2003</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>983</v>
-      </c>
-      <c r="C19" s="26" t="s">
+      <c r="B19" s="29" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26" t="s">
-        <v>984</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>985</v>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F19" s="29" t="s">
+        <v>1008</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="25" t="n">
         <v>2004</v>
       </c>
-      <c r="B20" s="26" t="s">
-        <v>986</v>
-      </c>
-      <c r="C20" s="26" t="s">
+      <c r="B20" s="29" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C20" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26" t="s">
-        <v>987</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>988</v>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>1011</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="25" t="n">
         <v>2006</v>
       </c>
-      <c r="B21" s="26" t="s">
-        <v>989</v>
-      </c>
-      <c r="C21" s="26" t="s">
+      <c r="B21" s="29" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C21" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26" t="s">
-        <v>990</v>
-      </c>
-      <c r="F21" s="26" t="s">
-        <v>991</v>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>1014</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="25" t="n">
         <v>2005</v>
       </c>
-      <c r="B22" s="26" t="s">
-        <v>992</v>
-      </c>
-      <c r="C22" s="26" t="s">
+      <c r="B22" s="29" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C22" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26" t="s">
-        <v>993</v>
-      </c>
-      <c r="F22" s="26" t="s">
-        <v>994</v>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29" t="s">
+        <v>1016</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>1017</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="25" t="n">
         <v>2018</v>
       </c>
-      <c r="B23" s="26" t="s">
-        <v>995</v>
-      </c>
-      <c r="C23" s="26" t="s">
+      <c r="B23" s="29" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C23" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26" t="s">
-        <v>996</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>997</v>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>1020</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="25" t="n">
         <v>2009</v>
       </c>
-      <c r="B24" s="26" t="s">
-        <v>998</v>
-      </c>
-      <c r="C24" s="26" t="s">
+      <c r="B24" s="29" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C24" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26" t="s">
-        <v>999</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>1000</v>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>1023</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="25" t="n">
         <v>2025</v>
       </c>
-      <c r="B25" s="26" t="s">
-        <v>1001</v>
-      </c>
-      <c r="C25" s="26" t="s">
+      <c r="B25" s="29" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C25" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26" t="s">
-        <v>1002</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>1003</v>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>1026</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="25" t="n">
         <v>2007</v>
       </c>
-      <c r="B26" s="26" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C26" s="26" t="s">
+      <c r="B26" s="29" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C26" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26" t="s">
-        <v>1005</v>
-      </c>
-      <c r="F26" s="26" t="s">
-        <v>1006</v>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>1029</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="25" t="n">
         <v>2019</v>
       </c>
-      <c r="B27" s="26" t="s">
-        <v>1007</v>
-      </c>
-      <c r="C27" s="26" t="s">
+      <c r="B27" s="29" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C27" s="29" t="s">
         <v>853</v>
       </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26" t="s">
-        <v>1008</v>
-      </c>
-      <c r="F27" s="26" t="s">
-        <v>1009</v>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>1032</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="25" t="n">
         <v>2031</v>
       </c>
-      <c r="B28" s="26" t="s">
-        <v>1010</v>
-      </c>
-      <c r="C28" s="26" t="s">
+      <c r="B28" s="29" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C28" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26" t="s">
-        <v>1011</v>
-      </c>
-      <c r="F28" s="26" t="s">
-        <v>1012</v>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>1035</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="25" t="n">
         <v>2030</v>
       </c>
-      <c r="B29" s="26" t="s">
-        <v>1013</v>
-      </c>
-      <c r="C29" s="26" t="s">
+      <c r="B29" s="29" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C29" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26" t="s">
-        <v>1014</v>
-      </c>
-      <c r="F29" s="26" t="s">
-        <v>1012</v>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>1035</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="25" t="n">
         <v>2033</v>
       </c>
-      <c r="B30" s="26" t="s">
-        <v>1015</v>
-      </c>
-      <c r="C30" s="26" t="s">
+      <c r="B30" s="29" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C30" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26" t="s">
-        <v>1016</v>
-      </c>
-      <c r="F30" s="26" t="s">
-        <v>1012</v>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>1035</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="25" t="n">
         <v>2032</v>
       </c>
-      <c r="B31" s="26" t="s">
-        <v>1017</v>
-      </c>
-      <c r="C31" s="26" t="s">
+      <c r="B31" s="29" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C31" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26" t="s">
-        <v>1018</v>
-      </c>
-      <c r="F31" s="26" t="s">
-        <v>1019</v>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>1042</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="25" t="n">
         <v>2026</v>
       </c>
-      <c r="B32" s="26" t="s">
-        <v>1020</v>
-      </c>
-      <c r="C32" s="26" t="s">
+      <c r="B32" s="29" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C32" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26" t="s">
-        <v>1021</v>
-      </c>
-      <c r="F32" s="26" t="s">
-        <v>1022</v>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F32" s="29" t="s">
+        <v>1045</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="25" t="n">
         <v>2027</v>
       </c>
-      <c r="B33" s="26" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C33" s="26" t="s">
+      <c r="B33" s="29" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C33" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26" t="s">
-        <v>1024</v>
-      </c>
-      <c r="F33" s="26" t="s">
-        <v>1022</v>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F33" s="29" t="s">
+        <v>1045</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="25" t="n">
         <v>2029</v>
       </c>
-      <c r="B34" s="26" t="s">
-        <v>1025</v>
-      </c>
-      <c r="C34" s="26" t="s">
+      <c r="B34" s="29" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C34" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26" t="s">
-        <v>1026</v>
-      </c>
-      <c r="F34" s="26" t="s">
-        <v>1027</v>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29" t="s">
+        <v>1049</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>1050</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="25" t="n">
         <v>2028</v>
       </c>
-      <c r="B35" s="26" t="s">
-        <v>1028</v>
-      </c>
-      <c r="C35" s="26" t="s">
+      <c r="B35" s="29" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C35" s="29" t="s">
         <v>875</v>
       </c>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26" t="s">
-        <v>1029</v>
-      </c>
-      <c r="F35" s="26" t="s">
-        <v>1030</v>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29" t="s">
+        <v>1052</v>
+      </c>
+      <c r="F35" s="29" t="s">
+        <v>1053</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="25" t="n">
         <v>2043</v>
       </c>
-      <c r="B36" s="26" t="s">
-        <v>1031</v>
-      </c>
-      <c r="C36" s="26" t="s">
+      <c r="B36" s="29" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C36" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D36" s="26" t="s">
+      <c r="D36" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E36" s="26" t="s">
-        <v>1032</v>
-      </c>
-      <c r="F36" s="26" t="s">
-        <v>1033</v>
+      <c r="E36" s="29" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>1056</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="25" t="n">
         <v>2040</v>
       </c>
-      <c r="B37" s="26" t="s">
-        <v>1034</v>
-      </c>
-      <c r="C37" s="26" t="s">
+      <c r="B37" s="29" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C37" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D37" s="26" t="s">
+      <c r="D37" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E37" s="26" t="s">
-        <v>1035</v>
-      </c>
-      <c r="F37" s="26" t="s">
-        <v>1036</v>
+      <c r="E37" s="29" t="s">
+        <v>1058</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>1059</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="25" t="n">
         <v>2035</v>
       </c>
-      <c r="B38" s="26" t="s">
-        <v>1037</v>
-      </c>
-      <c r="C38" s="26" t="s">
+      <c r="B38" s="29" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C38" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D38" s="26" t="s">
+      <c r="D38" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E38" s="26" t="s">
-        <v>1038</v>
-      </c>
-      <c r="F38" s="26" t="s">
-        <v>1039</v>
+      <c r="E38" s="29" t="s">
+        <v>1061</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>1062</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="25" t="n">
         <v>2041</v>
       </c>
-      <c r="B39" s="26" t="s">
-        <v>1040</v>
-      </c>
-      <c r="C39" s="26" t="s">
+      <c r="B39" s="29" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C39" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D39" s="26" t="s">
+      <c r="D39" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E39" s="26" t="s">
-        <v>1041</v>
-      </c>
-      <c r="F39" s="26" t="s">
-        <v>1042</v>
+      <c r="E39" s="29" t="s">
+        <v>1064</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>1065</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="25" t="n">
         <v>2042</v>
       </c>
-      <c r="B40" s="26" t="s">
-        <v>1043</v>
-      </c>
-      <c r="C40" s="26" t="s">
+      <c r="B40" s="29" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C40" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D40" s="26" t="s">
+      <c r="D40" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E40" s="26" t="s">
-        <v>1044</v>
-      </c>
-      <c r="F40" s="26" t="s">
-        <v>1042</v>
+      <c r="E40" s="29" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F40" s="29" t="s">
+        <v>1065</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="25" t="n">
         <v>2044</v>
       </c>
-      <c r="B41" s="26" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C41" s="26" t="s">
+      <c r="B41" s="29" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C41" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D41" s="26" t="s">
+      <c r="D41" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E41" s="26" t="s">
-        <v>1046</v>
-      </c>
-      <c r="F41" s="26" t="s">
-        <v>1047</v>
+      <c r="E41" s="29" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>1070</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="25" t="n">
         <v>2036</v>
       </c>
-      <c r="B42" s="26" t="s">
-        <v>1048</v>
-      </c>
-      <c r="C42" s="26" t="s">
+      <c r="B42" s="29" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C42" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D42" s="26" t="s">
+      <c r="D42" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E42" s="26" t="s">
-        <v>1049</v>
-      </c>
-      <c r="F42" s="26" t="s">
-        <v>1050</v>
+      <c r="E42" s="29" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>1073</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="25" t="n">
         <v>2034</v>
       </c>
-      <c r="B43" s="26" t="s">
-        <v>1051</v>
-      </c>
-      <c r="C43" s="26" t="s">
+      <c r="B43" s="29" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C43" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D43" s="26" t="s">
+      <c r="D43" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E43" s="26" t="s">
-        <v>1052</v>
-      </c>
-      <c r="F43" s="26" t="s">
-        <v>1053</v>
+      <c r="E43" s="29" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>1076</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="25" t="n">
         <v>2037</v>
       </c>
-      <c r="B44" s="26" t="s">
-        <v>1054</v>
-      </c>
-      <c r="C44" s="26" t="s">
+      <c r="B44" s="29" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C44" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D44" s="26" t="s">
+      <c r="D44" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E44" s="26" t="s">
-        <v>1055</v>
-      </c>
-      <c r="F44" s="26" t="s">
-        <v>1056</v>
+      <c r="E44" s="29" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>1079</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="25" t="n">
         <v>2038</v>
       </c>
-      <c r="B45" s="26" t="s">
-        <v>1057</v>
-      </c>
-      <c r="C45" s="26" t="s">
+      <c r="B45" s="29" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C45" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D45" s="26" t="s">
+      <c r="D45" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E45" s="26" t="s">
-        <v>1058</v>
-      </c>
-      <c r="F45" s="26" t="s">
-        <v>1056</v>
+      <c r="E45" s="29" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>1079</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="25" t="n">
         <v>2039</v>
       </c>
-      <c r="B46" s="26" t="s">
-        <v>1059</v>
-      </c>
-      <c r="C46" s="26" t="s">
+      <c r="B46" s="29" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C46" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D46" s="26" t="s">
+      <c r="D46" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E46" s="26" t="s">
-        <v>1060</v>
-      </c>
-      <c r="F46" s="26" t="s">
-        <v>1056</v>
+      <c r="E46" s="29" t="s">
+        <v>1083</v>
+      </c>
+      <c r="F46" s="29" t="s">
+        <v>1079</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="25" t="n">
         <v>2045</v>
       </c>
-      <c r="B47" s="26" t="s">
-        <v>1061</v>
-      </c>
-      <c r="C47" s="26" t="s">
+      <c r="B47" s="29" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C47" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="D47" s="26" t="s">
+      <c r="D47" s="29" t="s">
         <v>758</v>
       </c>
-      <c r="E47" s="26" t="s">
-        <v>1062</v>
-      </c>
-      <c r="F47" s="26" t="s">
-        <v>1063</v>
+      <c r="E47" s="29" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F47" s="29" t="s">
+        <v>1086</v>
       </c>
     </row>
   </sheetData>
@@ -20655,22 +21030,22 @@
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
-        <v>1064</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>1065</v>
+      <c r="A1" s="29" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>1088</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>1066</v>
-      </c>
-      <c r="B2" s="27" t="n">
+      <c r="A2" s="29" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B2" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>